<commit_message>
Remove unnecessary source_id field from forms
</commit_message>
<xml_diff>
--- a/case-id/forms/app/register_case.xlsx
+++ b/case-id/forms/app/register_case.xlsx
@@ -233,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -290,12 +290,6 @@
   </si>
   <si>
     <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source ID</t>
   </si>
   <si>
     <t xml:space="preserve">contact</t>
@@ -844,14 +838,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -933,7 +927,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>19</v>
@@ -941,19 +935,22 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -961,82 +958,65 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="4"/>
+      <c r="D15" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:I10000 A27:B27 A2:C26 D2:F13 A28:F10000 D17:F27 E14:F16">
+  <conditionalFormatting sqref="H2:I9999 A26:B26 A5:C25 D5:F12 A27:F9999 D16:F26 E13:F15 A2:F4">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -1053,44 +1033,44 @@
       <formula>AND(ISBLANK($A2), NOT(ISBLANK(A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B10000">
+  <conditionalFormatting sqref="B2:B9999">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C10000 C2:C26">
+  <conditionalFormatting sqref="C27:C9999 C2:C25">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10000">
+  <conditionalFormatting sqref="H2:H9999">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A2="calculate", ISBLANK(H2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
+  <conditionalFormatting sqref="C26">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$A27="begin_group"</formula>
+      <formula>$A26="begin_group"</formula>
     </cfRule>
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$A27="end_group"</formula>
+      <formula>$A26="end_group"</formula>
     </cfRule>
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$A27="begin_repeat"</formula>
+      <formula>$A26="begin_repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$A27="end_repeat"</formula>
+      <formula>$A26="end_repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK($A27), NOT(ISBLANK(C27)))</formula>
+      <formula>AND(ISBLANK($A26), NOT(ISBLANK(C26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
+  <conditionalFormatting sqref="C26">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C27),NOT(OR(ISBLANK($A27),$A27="calculate")))</formula>
+      <formula>AND(ISBLANK(C26),NOT(OR(ISBLANK($A26),$A26="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10000">
+  <conditionalFormatting sqref="G2:G9999">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -1112,7 +1092,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1015" type="list">
+    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1014" type="list">
       <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1149,37 +1129,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250213162705</v>
+        <v>20250214130852</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add basic task configuration (#18)
</commit_message>
<xml_diff>
--- a/case-id/forms/app/register_case.xlsx
+++ b/case-id/forms/app/register_case.xlsx
@@ -233,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -290,12 +290,6 @@
   </si>
   <si>
     <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source ID</t>
   </si>
   <si>
     <t xml:space="preserve">contact</t>
@@ -844,14 +838,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -933,7 +927,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>19</v>
@@ -941,19 +935,22 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -961,82 +958,65 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="4"/>
+      <c r="D15" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:I10000 A27:B27 A2:C26 D2:F13 A28:F10000 D17:F27 E14:F16">
+  <conditionalFormatting sqref="H2:I9999 A26:B26 A5:C25 D5:F12 A27:F9999 D16:F26 E13:F15 A2:F4">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -1053,44 +1033,44 @@
       <formula>AND(ISBLANK($A2), NOT(ISBLANK(A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B10000">
+  <conditionalFormatting sqref="B2:B9999">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C10000 C2:C26">
+  <conditionalFormatting sqref="C27:C9999 C2:C25">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10000">
+  <conditionalFormatting sqref="H2:H9999">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A2="calculate", ISBLANK(H2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
+  <conditionalFormatting sqref="C26">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$A27="begin_group"</formula>
+      <formula>$A26="begin_group"</formula>
     </cfRule>
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$A27="end_group"</formula>
+      <formula>$A26="end_group"</formula>
     </cfRule>
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$A27="begin_repeat"</formula>
+      <formula>$A26="begin_repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$A27="end_repeat"</formula>
+      <formula>$A26="end_repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK($A27), NOT(ISBLANK(C27)))</formula>
+      <formula>AND(ISBLANK($A26), NOT(ISBLANK(C26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
+  <conditionalFormatting sqref="C26">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C27),NOT(OR(ISBLANK($A27),$A27="calculate")))</formula>
+      <formula>AND(ISBLANK(C26),NOT(OR(ISBLANK($A26),$A26="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10000">
+  <conditionalFormatting sqref="G2:G9999">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A2="begin_group"</formula>
     </cfRule>
@@ -1112,7 +1092,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1015" type="list">
+    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1014" type="list">
       <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1149,37 +1129,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250213162705</v>
+        <v>20250214130852</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>